<commit_message>
move tokyo eye shot to shadowrun
</commit_message>
<xml_diff>
--- a/fantasy-file/checklist.xlsx
+++ b/fantasy-file/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/fantasy-file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502E3B10-DB4B-3B40-8170-9933E381852F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F22C8DE-5820-734B-ACD0-A695DA7F3BE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{E5AEC0A0-1D25-3F4F-A8D5-50372A80A5C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="158">
   <si>
     <t>year</t>
   </si>
@@ -384,15 +384,6 @@
   </si>
   <si>
     <t>fantasy_rpg_quiz_4.jpg</t>
-  </si>
-  <si>
-    <t>TOKYO EYE‐SHOT シャドウランシティファイル</t>
-  </si>
-  <si>
-    <t>Tokyo Eye Shot: Shadowrun City File</t>
-  </si>
-  <si>
-    <t>shadowrun_tokyo_eye_shot.jpg</t>
   </si>
   <si>
     <t>product_type</t>
@@ -883,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C3CF34-BE94-804A-8259-9F58E98E2002}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -916,10 +907,10 @@
         <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -939,10 +930,10 @@
         <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -962,10 +953,10 @@
         <v>81</v>
       </c>
       <c r="F3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -985,10 +976,10 @@
         <v>82</v>
       </c>
       <c r="F4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1008,10 +999,10 @@
         <v>83</v>
       </c>
       <c r="F5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1031,10 +1022,10 @@
         <v>84</v>
       </c>
       <c r="F6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1054,10 +1045,10 @@
         <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1077,10 +1068,10 @@
         <v>115</v>
       </c>
       <c r="F8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1100,10 +1091,10 @@
         <v>86</v>
       </c>
       <c r="F9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1123,10 +1114,10 @@
         <v>85</v>
       </c>
       <c r="F10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1146,10 +1137,10 @@
         <v>88</v>
       </c>
       <c r="F11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1169,10 +1160,10 @@
         <v>90</v>
       </c>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1192,10 +1183,10 @@
         <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1215,10 +1206,10 @@
         <v>112</v>
       </c>
       <c r="F14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1238,10 +1229,10 @@
         <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1261,10 +1252,10 @@
         <v>97</v>
       </c>
       <c r="F16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1284,10 +1275,10 @@
         <v>93</v>
       </c>
       <c r="F17" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1307,10 +1298,10 @@
         <v>100</v>
       </c>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1330,10 +1321,10 @@
         <v>101</v>
       </c>
       <c r="F19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1353,10 +1344,10 @@
         <v>92</v>
       </c>
       <c r="F20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1376,10 +1367,10 @@
         <v>113</v>
       </c>
       <c r="F21" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1399,10 +1390,10 @@
         <v>102</v>
       </c>
       <c r="F22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1422,10 +1413,10 @@
         <v>96</v>
       </c>
       <c r="F23" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1445,10 +1436,10 @@
         <v>95</v>
       </c>
       <c r="F24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1468,10 +1459,10 @@
         <v>99</v>
       </c>
       <c r="F25" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1491,10 +1482,10 @@
         <v>98</v>
       </c>
       <c r="F26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1514,10 +1505,10 @@
         <v>94</v>
       </c>
       <c r="F27" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1537,10 +1528,10 @@
         <v>104</v>
       </c>
       <c r="F28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1560,10 +1551,10 @@
         <v>114</v>
       </c>
       <c r="F29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1583,10 +1574,10 @@
         <v>116</v>
       </c>
       <c r="F30" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1606,10 +1597,10 @@
         <v>103</v>
       </c>
       <c r="F31" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1629,10 +1620,10 @@
         <v>106</v>
       </c>
       <c r="F32" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1652,10 +1643,10 @@
         <v>105</v>
       </c>
       <c r="F33" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1675,10 +1666,10 @@
         <v>109</v>
       </c>
       <c r="F34" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1698,10 +1689,10 @@
         <v>110</v>
       </c>
       <c r="F35" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1721,10 +1712,10 @@
         <v>108</v>
       </c>
       <c r="F36" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1744,10 +1735,10 @@
         <v>107</v>
       </c>
       <c r="F37" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1767,32 +1758,11 @@
         <v>111</v>
       </c>
       <c r="F38" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>1995</v>
-      </c>
-      <c r="B39" t="s">
-        <v>117</v>
-      </c>
-      <c r="C39" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" t="s">
-        <v>119</v>
-      </c>
-      <c r="F39" t="s">
-        <v>121</v>
-      </c>
-      <c r="G39" s="2"/>
+        <v>151</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>